<commit_message>
all images and tables correct now
</commit_message>
<xml_diff>
--- a/Tags.xlsx
+++ b/Tags.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\XHQPRDCGY011\Production_Python_Scripts\Produced Gas Daily Report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://suncor-my.sharepoint.com/personal/mobeaulieu_suncor_com2/Documents/Documents/python_projects_local/pg_script/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45D2F0E-55A9-46E4-9B71-EF3336E11713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38290" yWindow="-110" windowWidth="38620" windowHeight="21100" tabRatio="753" activeTab="2" xr2:uid="{702E8C0B-36B5-40C9-B840-0E41148BC5C0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="753" xr2:uid="{702E8C0B-36B5-40C9-B840-0E41148BC5C0}"/>
   </bookViews>
   <sheets>
     <sheet name="tags_well" sheetId="2" r:id="rId1"/>
@@ -3760,9 +3760,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3800,7 +3800,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3906,7 +3906,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -4048,7 +4048,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4058,18 +4058,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A00ACC3C-6C5D-4438-9240-37A1B7AAAE31}">
   <dimension ref="A1:E296"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.75" customWidth="1"/>
     <col min="2" max="4" width="29.25" customWidth="1"/>
-    <col min="5" max="5" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4086,7 +4086,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>770</v>
       </c>
@@ -4103,7 +4103,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>770</v>
       </c>
@@ -4120,7 +4120,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>770</v>
       </c>
@@ -4137,7 +4137,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>770</v>
       </c>
@@ -4154,7 +4154,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>770</v>
       </c>
@@ -4171,7 +4171,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>770</v>
       </c>
@@ -4188,7 +4188,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>770</v>
       </c>
@@ -4205,7 +4205,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>770</v>
       </c>
@@ -4222,7 +4222,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>770</v>
       </c>
@@ -4239,7 +4239,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>770</v>
       </c>
@@ -4256,7 +4256,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>770</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>770</v>
       </c>
@@ -4290,7 +4290,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>770</v>
       </c>
@@ -4307,7 +4307,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>770</v>
       </c>
@@ -4324,7 +4324,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>770</v>
       </c>
@@ -4341,7 +4341,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>770</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>770</v>
       </c>
@@ -4375,7 +4375,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>770</v>
       </c>
@@ -4392,7 +4392,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>770</v>
       </c>
@@ -4409,7 +4409,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>770</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>770</v>
       </c>
@@ -4443,7 +4443,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>770</v>
       </c>
@@ -4460,7 +4460,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>770</v>
       </c>
@@ -4477,7 +4477,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>770</v>
       </c>
@@ -4494,7 +4494,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>770</v>
       </c>
@@ -4511,7 +4511,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>770</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>770</v>
       </c>
@@ -4545,7 +4545,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>770</v>
       </c>
@@ -4562,7 +4562,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>770</v>
       </c>
@@ -4579,7 +4579,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>770</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>770</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>771</v>
       </c>
@@ -4630,7 +4630,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>771</v>
       </c>
@@ -4647,7 +4647,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>771</v>
       </c>
@@ -4664,7 +4664,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>771</v>
       </c>
@@ -4681,7 +4681,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>771</v>
       </c>
@@ -4698,7 +4698,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>771</v>
       </c>
@@ -4715,7 +4715,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>771</v>
       </c>
@@ -4732,7 +4732,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>771</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>771</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>771</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>771</v>
       </c>
@@ -4800,7 +4800,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>771</v>
       </c>
@@ -4817,7 +4817,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>771</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>771</v>
       </c>
@@ -4851,7 +4851,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>771</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>772</v>
       </c>
@@ -4885,7 +4885,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>772</v>
       </c>
@@ -4902,7 +4902,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>772</v>
       </c>
@@ -4919,7 +4919,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>772</v>
       </c>
@@ -4936,7 +4936,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>772</v>
       </c>
@@ -4953,7 +4953,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>772</v>
       </c>
@@ -4970,7 +4970,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>772</v>
       </c>
@@ -4987,7 +4987,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>772</v>
       </c>
@@ -5004,7 +5004,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>772</v>
       </c>
@@ -5021,7 +5021,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>772</v>
       </c>
@@ -5038,7 +5038,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>772</v>
       </c>
@@ -5055,7 +5055,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>772</v>
       </c>
@@ -5072,7 +5072,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>772</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>772</v>
       </c>
@@ -5106,7 +5106,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>772</v>
       </c>
@@ -5123,7 +5123,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>772</v>
       </c>
@@ -5140,7 +5140,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>754</v>
       </c>
@@ -5157,7 +5157,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>754</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>754</v>
       </c>
@@ -5191,7 +5191,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>754</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>754</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>754</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>754</v>
       </c>
@@ -5259,7 +5259,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>754</v>
       </c>
@@ -5276,7 +5276,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>754</v>
       </c>
@@ -5293,7 +5293,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>754</v>
       </c>
@@ -5310,7 +5310,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>754</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>754</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>754</v>
       </c>
@@ -5361,7 +5361,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>754</v>
       </c>
@@ -5378,7 +5378,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>754</v>
       </c>
@@ -5395,7 +5395,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>754</v>
       </c>
@@ -5412,7 +5412,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>754</v>
       </c>
@@ -5429,7 +5429,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>754</v>
       </c>
@@ -5446,7 +5446,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>754</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>754</v>
       </c>
@@ -5480,7 +5480,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>754</v>
       </c>
@@ -5497,7 +5497,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>754</v>
       </c>
@@ -5514,7 +5514,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>754</v>
       </c>
@@ -5531,7 +5531,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>754</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>754</v>
       </c>
@@ -5565,7 +5565,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>754</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>754</v>
       </c>
@@ -5599,7 +5599,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>754</v>
       </c>
@@ -5616,7 +5616,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>754</v>
       </c>
@@ -5633,7 +5633,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>754</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>754</v>
       </c>
@@ -5667,7 +5667,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>754</v>
       </c>
@@ -5684,7 +5684,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>754</v>
       </c>
@@ -5701,7 +5701,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>754</v>
       </c>
@@ -5718,7 +5718,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>754</v>
       </c>
@@ -5735,7 +5735,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>754</v>
       </c>
@@ -5752,7 +5752,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>754</v>
       </c>
@@ -5769,7 +5769,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>754</v>
       </c>
@@ -5786,7 +5786,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>754</v>
       </c>
@@ -5803,7 +5803,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>754</v>
       </c>
@@ -5820,7 +5820,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>754</v>
       </c>
@@ -5837,7 +5837,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>754</v>
       </c>
@@ -5854,7 +5854,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>754</v>
       </c>
@@ -5871,7 +5871,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>754</v>
       </c>
@@ -5888,7 +5888,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>754</v>
       </c>
@@ -5905,7 +5905,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>754</v>
       </c>
@@ -5922,7 +5922,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>754</v>
       </c>
@@ -5939,7 +5939,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>754</v>
       </c>
@@ -5956,7 +5956,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>754</v>
       </c>
@@ -5973,7 +5973,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>754</v>
       </c>
@@ -5990,7 +5990,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>754</v>
       </c>
@@ -6007,7 +6007,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>754</v>
       </c>
@@ -6024,7 +6024,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>754</v>
       </c>
@@ -6041,7 +6041,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>754</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>754</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>754</v>
       </c>
@@ -6092,7 +6092,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>754</v>
       </c>
@@ -6109,7 +6109,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>754</v>
       </c>
@@ -6126,7 +6126,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>754</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>754</v>
       </c>
@@ -6160,7 +6160,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>754</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>754</v>
       </c>
@@ -6194,7 +6194,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>754</v>
       </c>
@@ -6211,7 +6211,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>754</v>
       </c>
@@ -6228,7 +6228,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>754</v>
       </c>
@@ -6245,7 +6245,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>754</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>754</v>
       </c>
@@ -6279,7 +6279,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>754</v>
       </c>
@@ -6296,7 +6296,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>754</v>
       </c>
@@ -6313,7 +6313,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>754</v>
       </c>
@@ -6330,7 +6330,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>754</v>
       </c>
@@ -6347,7 +6347,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>754</v>
       </c>
@@ -6364,7 +6364,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>754</v>
       </c>
@@ -6381,7 +6381,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>754</v>
       </c>
@@ -6398,7 +6398,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>754</v>
       </c>
@@ -6415,7 +6415,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>754</v>
       </c>
@@ -6432,7 +6432,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>754</v>
       </c>
@@ -6449,7 +6449,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>754</v>
       </c>
@@ -6466,7 +6466,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>754</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>754</v>
       </c>
@@ -6500,7 +6500,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>754</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>754</v>
       </c>
@@ -6534,7 +6534,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>754</v>
       </c>
@@ -6551,7 +6551,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>754</v>
       </c>
@@ -6568,7 +6568,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>754</v>
       </c>
@@ -6585,7 +6585,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>754</v>
       </c>
@@ -6602,7 +6602,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>754</v>
       </c>
@@ -6619,7 +6619,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>754</v>
       </c>
@@ -6636,7 +6636,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>754</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>754</v>
       </c>
@@ -6670,7 +6670,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>754</v>
       </c>
@@ -6687,7 +6687,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>754</v>
       </c>
@@ -6704,7 +6704,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>754</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>1196</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>754</v>
       </c>
@@ -6738,7 +6738,7 @@
         <v>1197</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>754</v>
       </c>
@@ -6755,7 +6755,7 @@
         <v>1198</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>754</v>
       </c>
@@ -6772,7 +6772,7 @@
         <v>1199</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>754</v>
       </c>
@@ -6789,7 +6789,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>754</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>1201</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>754</v>
       </c>
@@ -6823,7 +6823,7 @@
         <v>1202</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>754</v>
       </c>
@@ -6840,7 +6840,7 @@
         <v>1203</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>773</v>
       </c>
@@ -6857,7 +6857,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>773</v>
       </c>
@@ -6874,7 +6874,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>773</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>773</v>
       </c>
@@ -6908,7 +6908,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>773</v>
       </c>
@@ -6925,7 +6925,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>773</v>
       </c>
@@ -6942,7 +6942,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>773</v>
       </c>
@@ -6959,7 +6959,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>773</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>773</v>
       </c>
@@ -6993,7 +6993,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>773</v>
       </c>
@@ -7010,7 +7010,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>773</v>
       </c>
@@ -7027,7 +7027,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>773</v>
       </c>
@@ -7044,7 +7044,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>773</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>773</v>
       </c>
@@ -7078,7 +7078,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" s="1" t="s">
         <v>774</v>
       </c>
@@ -7095,7 +7095,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" s="1" t="s">
         <v>774</v>
       </c>
@@ -7112,7 +7112,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" s="1" t="s">
         <v>774</v>
       </c>
@@ -7129,7 +7129,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" s="1" t="s">
         <v>774</v>
       </c>
@@ -7146,7 +7146,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" s="1" t="s">
         <v>774</v>
       </c>
@@ -7163,7 +7163,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" s="1" t="s">
         <v>774</v>
       </c>
@@ -7180,7 +7180,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" s="1" t="s">
         <v>774</v>
       </c>
@@ -7197,7 +7197,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" s="1" t="s">
         <v>774</v>
       </c>
@@ -7214,7 +7214,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" s="1" t="s">
         <v>774</v>
       </c>
@@ -7231,7 +7231,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>774</v>
       </c>
@@ -7248,7 +7248,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" s="1" t="s">
         <v>774</v>
       </c>
@@ -7265,7 +7265,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" s="1" t="s">
         <v>774</v>
       </c>
@@ -7282,7 +7282,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" s="1" t="s">
         <v>774</v>
       </c>
@@ -7299,7 +7299,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" s="1" t="s">
         <v>774</v>
       </c>
@@ -7316,7 +7316,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" s="1" t="s">
         <v>774</v>
       </c>
@@ -7333,7 +7333,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
         <v>775</v>
       </c>
@@ -7350,7 +7350,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" s="1" t="s">
         <v>775</v>
       </c>
@@ -7367,7 +7367,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" s="1" t="s">
         <v>775</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" s="1" t="s">
         <v>775</v>
       </c>
@@ -7401,7 +7401,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" s="1" t="s">
         <v>775</v>
       </c>
@@ -7418,7 +7418,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" s="1" t="s">
         <v>775</v>
       </c>
@@ -7435,7 +7435,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" s="1" t="s">
         <v>775</v>
       </c>
@@ -7452,7 +7452,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" s="1" t="s">
         <v>775</v>
       </c>
@@ -7469,7 +7469,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" s="1" t="s">
         <v>775</v>
       </c>
@@ -7486,7 +7486,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" s="1" t="s">
         <v>775</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" s="1" t="s">
         <v>775</v>
       </c>
@@ -7520,7 +7520,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A204" s="1" t="s">
         <v>775</v>
       </c>
@@ -7537,7 +7537,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" s="1" t="s">
         <v>775</v>
       </c>
@@ -7554,7 +7554,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
         <v>775</v>
       </c>
@@ -7571,7 +7571,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" s="1" t="s">
         <v>775</v>
       </c>
@@ -7588,7 +7588,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>775</v>
       </c>
@@ -7605,7 +7605,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" s="1" t="s">
         <v>775</v>
       </c>
@@ -7622,7 +7622,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" s="1" t="s">
         <v>775</v>
       </c>
@@ -7639,7 +7639,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" s="1" t="s">
         <v>775</v>
       </c>
@@ -7656,7 +7656,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" s="1" t="s">
         <v>810</v>
       </c>
@@ -7673,7 +7673,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" s="1" t="s">
         <v>810</v>
       </c>
@@ -7690,7 +7690,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" s="1" t="s">
         <v>810</v>
       </c>
@@ -7707,7 +7707,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" s="1" t="s">
         <v>810</v>
       </c>
@@ -7724,7 +7724,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" s="1" t="s">
         <v>810</v>
       </c>
@@ -7741,7 +7741,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" s="1" t="s">
         <v>810</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" s="1" t="s">
         <v>810</v>
       </c>
@@ -7775,7 +7775,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" s="1" t="s">
         <v>810</v>
       </c>
@@ -7792,7 +7792,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" s="1" t="s">
         <v>878</v>
       </c>
@@ -7809,7 +7809,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" s="1" t="s">
         <v>878</v>
       </c>
@@ -7826,7 +7826,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" s="1" t="s">
         <v>878</v>
       </c>
@@ -7843,7 +7843,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" s="1" t="s">
         <v>878</v>
       </c>
@@ -7860,7 +7860,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" s="1" t="s">
         <v>878</v>
       </c>
@@ -7877,7 +7877,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" s="1" t="s">
         <v>878</v>
       </c>
@@ -7894,7 +7894,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" s="1" t="s">
         <v>878</v>
       </c>
@@ -7911,7 +7911,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" s="1" t="s">
         <v>878</v>
       </c>
@@ -7928,7 +7928,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" s="1" t="s">
         <v>878</v>
       </c>
@@ -7945,7 +7945,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" s="1" t="s">
         <v>878</v>
       </c>
@@ -7962,7 +7962,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" s="1" t="s">
         <v>878</v>
       </c>
@@ -7979,7 +7979,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" s="1" t="s">
         <v>878</v>
       </c>
@@ -7996,7 +7996,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" s="1" t="s">
         <v>878</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" s="1" t="s">
         <v>878</v>
       </c>
@@ -8030,7 +8030,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" s="1" t="s">
         <v>878</v>
       </c>
@@ -8047,7 +8047,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" s="1" t="s">
         <v>771</v>
       </c>
@@ -8064,7 +8064,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" s="1" t="s">
         <v>771</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" s="1" t="s">
         <v>771</v>
       </c>
@@ -8098,7 +8098,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" s="1" t="s">
         <v>771</v>
       </c>
@@ -8115,7 +8115,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" s="1" t="s">
         <v>771</v>
       </c>
@@ -8132,7 +8132,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" s="1" t="s">
         <v>771</v>
       </c>
@@ -8149,7 +8149,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" s="1" t="s">
         <v>771</v>
       </c>
@@ -8166,7 +8166,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" s="1" t="s">
         <v>771</v>
       </c>
@@ -8183,7 +8183,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" s="1" t="s">
         <v>771</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" s="1" t="s">
         <v>771</v>
       </c>
@@ -8217,7 +8217,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" s="1" t="s">
         <v>771</v>
       </c>
@@ -8234,7 +8234,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" s="1" t="s">
         <v>771</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" s="1" t="s">
         <v>771</v>
       </c>
@@ -8268,7 +8268,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" s="1" t="s">
         <v>771</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" s="1" t="s">
         <v>771</v>
       </c>
@@ -8302,7 +8302,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" s="1" t="s">
         <v>771</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" s="1" t="s">
         <v>771</v>
       </c>
@@ -8336,7 +8336,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" s="1" t="s">
         <v>771</v>
       </c>
@@ -8353,7 +8353,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" s="1" t="s">
         <v>771</v>
       </c>
@@ -8370,7 +8370,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" s="1" t="s">
         <v>771</v>
       </c>
@@ -8387,7 +8387,7 @@
         <v>1039</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" s="1" t="s">
         <v>771</v>
       </c>
@@ -8404,7 +8404,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" s="1" t="s">
         <v>771</v>
       </c>
@@ -8421,7 +8421,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A257" s="1" t="s">
         <v>771</v>
       </c>
@@ -8438,7 +8438,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A258" s="1" t="s">
         <v>771</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A259" s="1" t="s">
         <v>771</v>
       </c>
@@ -8472,7 +8472,7 @@
         <v>1044</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A260" s="1" t="s">
         <v>771</v>
       </c>
@@ -8489,7 +8489,7 @@
         <v>1045</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A261" s="1" t="s">
         <v>771</v>
       </c>
@@ -8506,7 +8506,7 @@
         <v>1046</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A262" s="1" t="s">
         <v>771</v>
       </c>
@@ -8523,7 +8523,7 @@
         <v>1047</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A263" s="1" t="s">
         <v>943</v>
       </c>
@@ -8540,7 +8540,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A264" s="1" t="s">
         <v>943</v>
       </c>
@@ -8557,7 +8557,7 @@
         <v>1058</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A265" s="1" t="s">
         <v>943</v>
       </c>
@@ -8574,7 +8574,7 @@
         <v>1059</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A266" s="1" t="s">
         <v>943</v>
       </c>
@@ -8591,7 +8591,7 @@
         <v>1060</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A267" s="1" t="s">
         <v>943</v>
       </c>
@@ -8608,7 +8608,7 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A268" s="1" t="s">
         <v>943</v>
       </c>
@@ -8625,7 +8625,7 @@
         <v>1062</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A269" s="1" t="s">
         <v>943</v>
       </c>
@@ -8642,7 +8642,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
         <v>943</v>
       </c>
@@ -8659,7 +8659,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A271" s="1" t="s">
         <v>943</v>
       </c>
@@ -8676,7 +8676,7 @@
         <v>1065</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A272" s="1" t="s">
         <v>943</v>
       </c>
@@ -8693,7 +8693,7 @@
         <v>1066</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A273" s="1" t="s">
         <v>943</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>1067</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A274" s="1" t="s">
         <v>943</v>
       </c>
@@ -8727,7 +8727,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A275" s="1" t="s">
         <v>943</v>
       </c>
@@ -8744,7 +8744,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A276" s="1" t="s">
         <v>943</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A277" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8778,7 +8778,7 @@
         <v>1154</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A278" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8795,7 +8795,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A279" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8812,7 +8812,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A280" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8829,7 +8829,7 @@
         <v>1157</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A281" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8846,7 +8846,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A282" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8863,7 +8863,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A283" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8880,7 +8880,7 @@
         <v>1160</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A284" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A285" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8914,7 +8914,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A286" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8931,7 +8931,7 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A287" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8948,7 +8948,7 @@
         <v>1164</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A289" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8982,7 +8982,7 @@
         <v>1166</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A290" s="1" t="s">
         <v>1020</v>
       </c>
@@ -8999,7 +8999,7 @@
         <v>1167</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A291" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9016,7 +9016,7 @@
         <v>1168</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A292" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>1169</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A293" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9050,7 +9050,7 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A294" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9067,7 +9067,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A295" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9084,7 +9084,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A296" s="1" t="s">
         <v>1020</v>
       </c>
@@ -9116,13 +9116,13 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" customWidth="1"/>
-    <col min="2" max="2" width="23.6640625" customWidth="1"/>
+    <col min="1" max="1" width="7.625" customWidth="1"/>
+    <col min="2" max="2" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9130,7 +9130,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>770</v>
       </c>
@@ -9138,7 +9138,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>754</v>
       </c>
@@ -9146,7 +9146,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>772</v>
       </c>
@@ -9154,7 +9154,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>773</v>
       </c>
@@ -9162,7 +9162,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>771</v>
       </c>
@@ -9170,7 +9170,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>774</v>
       </c>
@@ -9178,7 +9178,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>775</v>
       </c>
@@ -9186,7 +9186,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>810</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>843</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>878</v>
       </c>
@@ -9202,7 +9202,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>941</v>
       </c>
@@ -9210,7 +9210,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>943</v>
       </c>
@@ -9218,7 +9218,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1020</v>
       </c>
@@ -9236,16 +9236,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B203113B-7083-444E-88FF-2733F819769F}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="20.9140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -9259,7 +9259,7 @@
         <v>845</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1208</v>
       </c>
@@ -9273,7 +9273,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>851</v>
       </c>
@@ -9287,7 +9287,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>849</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1206</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>850</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1204</v>
       </c>
@@ -9343,7 +9343,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>1194</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1195</v>
       </c>
@@ -9371,7 +9371,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>852</v>
       </c>
@@ -9385,7 +9385,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>844</v>
       </c>
@@ -9399,7 +9399,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>846</v>
       </c>
@@ -9413,7 +9413,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1205</v>
       </c>
@@ -9427,7 +9427,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1207</v>
       </c>
@@ -9441,7 +9441,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>853</v>
       </c>

</xml_diff>